<commit_message>
some changes, returned v2 to the repo
</commit_message>
<xml_diff>
--- a/v3/template.xlsx
+++ b/v3/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akha/Documents/api_excel/v3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FE04A3-BE87-4449-BEBC-E4F016A28BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7004842E-1678-E946-B75D-B782BE69A170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52800" yWindow="500" windowWidth="19200" windowHeight="19500" tabRatio="505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REESTR" sheetId="1" r:id="rId1"/>
@@ -883,9 +883,6 @@
     <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="4" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -895,6 +892,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1302,8 +1302,8 @@
   </sheetPr>
   <dimension ref="A1:R322"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="137" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1472,8 +1472,8 @@
       <c r="H10" s="67"/>
       <c r="I10" s="66"/>
       <c r="J10" s="29"/>
-      <c r="K10" s="77"/>
-      <c r="L10" s="77"/>
+      <c r="K10" s="81"/>
+      <c r="L10" s="81"/>
       <c r="M10" s="29"/>
     </row>
     <row r="11" spans="1:13" ht="19" thickBot="1" x14ac:dyDescent="0.25">
@@ -1500,16 +1500,16 @@
       <c r="J12" s="52"/>
     </row>
     <row r="13" spans="1:13" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F13" s="79" t="s">
+      <c r="F13" s="78" t="s">
         <v>107</v>
       </c>
-      <c r="G13" s="79" t="s">
+      <c r="G13" s="78" t="s">
         <v>106</v>
       </c>
-      <c r="H13" s="80" t="s">
+      <c r="H13" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="I13" s="81" t="s">
+      <c r="I13" s="80" t="s">
         <v>3</v>
       </c>
       <c r="M13" s="32"/>
@@ -1535,7 +1535,7 @@
         <v>4</v>
       </c>
       <c r="G15" s="39"/>
-      <c r="H15" s="78">
+      <c r="H15" s="77">
         <f>SUM(H17:H122)</f>
         <v>0</v>
       </c>
@@ -5228,8 +5228,8 @@
   <mergeCells count="1">
     <mergeCell ref="K10:L10"/>
   </mergeCells>
-  <pageMargins left="3" right="1" top="1" bottom="1" header="0" footer="1"/>
-  <pageSetup paperSize="9" scale="40" orientation="portrait" useFirstPageNumber="1" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageMargins left="1" right="0.2" top="0.2" bottom="0.2" header="0" footer="0.2"/>
+  <pageSetup paperSize="9" scale="60" orientation="portrait" useFirstPageNumber="1" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;12&amp;K000000Группа компаний «Шар Құрылыс»&amp;R&amp;K000000Дата и время печати  &amp;D &amp;T</oddFooter>
   </headerFooter>
@@ -5240,7 +5240,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:K49"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
updates to add_coordinators in v3
</commit_message>
<xml_diff>
--- a/v3/template.xlsx
+++ b/v3/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akha/Documents/api_excel/v3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7004842E-1678-E946-B75D-B782BE69A170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4A528B-34F9-5544-ADC6-15A771FFFE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="500" windowWidth="38400" windowHeight="21100" tabRatio="505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="500" windowWidth="38400" windowHeight="19500" tabRatio="505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REESTR" sheetId="1" r:id="rId1"/>
@@ -511,7 +511,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -689,11 +689,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="mediumDashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="mediumDashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -883,7 +901,6 @@
     <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="4" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -896,6 +913,19 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="4" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="14" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="14" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1303,7 +1333,7 @@
   <dimension ref="A1:R322"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1389,7 +1419,7 @@
       <c r="L4" s="44"/>
       <c r="M4" s="29"/>
     </row>
-    <row r="5" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="19" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="44"/>
       <c r="B5" s="45"/>
       <c r="C5" s="44"/>
@@ -1412,10 +1442,10 @@
       <c r="A6" s="44"/>
       <c r="B6" s="45"/>
       <c r="C6" s="44"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="67"/>
-      <c r="I6" s="66"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="84"/>
+      <c r="I6" s="83"/>
       <c r="J6" s="44"/>
       <c r="K6" s="44"/>
       <c r="L6" s="44"/>
@@ -1436,14 +1466,14 @@
       <c r="L7" s="52"/>
       <c r="M7" s="29"/>
     </row>
-    <row r="8" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="19" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="52"/>
       <c r="B8" s="45"/>
       <c r="C8" s="52"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="66"/>
+      <c r="F8" s="85"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="87"/>
+      <c r="I8" s="86"/>
       <c r="K8" s="52"/>
       <c r="L8" s="52"/>
       <c r="M8" s="29"/>
@@ -1472,8 +1502,8 @@
       <c r="H10" s="67"/>
       <c r="I10" s="66"/>
       <c r="J10" s="29"/>
-      <c r="K10" s="81"/>
-      <c r="L10" s="81"/>
+      <c r="K10" s="80"/>
+      <c r="L10" s="80"/>
       <c r="M10" s="29"/>
     </row>
     <row r="11" spans="1:13" ht="19" thickBot="1" x14ac:dyDescent="0.25">
@@ -1500,16 +1530,16 @@
       <c r="J12" s="52"/>
     </row>
     <row r="13" spans="1:13" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F13" s="78" t="s">
+      <c r="F13" s="77" t="s">
         <v>107</v>
       </c>
-      <c r="G13" s="78" t="s">
+      <c r="G13" s="77" t="s">
         <v>106</v>
       </c>
-      <c r="H13" s="79" t="s">
+      <c r="H13" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="I13" s="80" t="s">
+      <c r="I13" s="79" t="s">
         <v>3</v>
       </c>
       <c r="M13" s="32"/>
@@ -1535,7 +1565,7 @@
         <v>4</v>
       </c>
       <c r="G15" s="39"/>
-      <c r="H15" s="77">
+      <c r="H15" s="81">
         <f>SUM(H17:H122)</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
updates  in v3: template.xlsx, scripts.py, inner_registry.py. Added firmen_und_objekten.py to realize the coordination structure.
</commit_message>
<xml_diff>
--- a/v3/template.xlsx
+++ b/v3/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akha/Documents/api_excel/v3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4A528B-34F9-5544-ADC6-15A771FFFE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78727B1A-D9C3-FF41-B26A-E7B77FD68119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="500" windowWidth="38400" windowHeight="19500" tabRatio="505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15900" tabRatio="505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REESTR" sheetId="1" r:id="rId1"/>
@@ -344,9 +344,6 @@
     <t>УТВЕРЖДАЮ</t>
   </si>
   <si>
-    <t>РЕЕСТР ПЛАТЕЖЕЙ №</t>
-  </si>
-  <si>
     <t>ЖК "Grand Victoria 2"</t>
   </si>
   <si>
@@ -360,6 +357,9 @@
   </si>
   <si>
     <t>Наименование контрагента</t>
+  </si>
+  <si>
+    <t>РЕЕСТР Платежей №</t>
   </si>
 </sst>
 </file>
@@ -701,7 +701,9 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="mediumDashed">
+        <color auto="1"/>
+      </top>
       <bottom style="mediumDashed">
         <color auto="1"/>
       </bottom>
@@ -711,7 +713,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -910,19 +912,15 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="4" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="14" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="14" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1333,7 +1331,7 @@
   <dimension ref="A1:R322"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1419,7 +1417,7 @@
       <c r="L4" s="44"/>
       <c r="M4" s="29"/>
     </row>
-    <row r="5" spans="1:13" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="44"/>
       <c r="B5" s="45"/>
       <c r="C5" s="44"/>
@@ -1438,42 +1436,38 @@
       <c r="L5" s="44"/>
       <c r="M5" s="29"/>
     </row>
-    <row r="6" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="44"/>
       <c r="B6" s="45"/>
       <c r="C6" s="44"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="84"/>
-      <c r="I6" s="83"/>
       <c r="J6" s="44"/>
       <c r="K6" s="44"/>
       <c r="L6" s="44"/>
       <c r="M6" s="29"/>
     </row>
-    <row r="7" spans="1:13" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="47" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="52"/>
       <c r="B7" s="45"/>
       <c r="C7" s="52"/>
-      <c r="F7" s="65" t="s">
-        <v>102</v>
-      </c>
-      <c r="G7" s="66"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="66"/>
+      <c r="F7" s="83" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" s="84"/>
+      <c r="H7" s="85"/>
+      <c r="I7" s="81"/>
       <c r="J7" s="52"/>
       <c r="K7" s="52"/>
       <c r="L7" s="52"/>
       <c r="M7" s="29"/>
     </row>
-    <row r="8" spans="1:13" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="52"/>
       <c r="B8" s="45"/>
       <c r="C8" s="52"/>
-      <c r="F8" s="85"/>
-      <c r="G8" s="86"/>
-      <c r="H8" s="87"/>
-      <c r="I8" s="86"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="81"/>
       <c r="K8" s="52"/>
       <c r="L8" s="52"/>
       <c r="M8" s="29"/>
@@ -1502,8 +1496,8 @@
       <c r="H10" s="67"/>
       <c r="I10" s="66"/>
       <c r="J10" s="29"/>
-      <c r="K10" s="80"/>
-      <c r="L10" s="80"/>
+      <c r="K10" s="82"/>
+      <c r="L10" s="82"/>
       <c r="M10" s="29"/>
     </row>
     <row r="11" spans="1:13" ht="19" thickBot="1" x14ac:dyDescent="0.25">
@@ -1531,10 +1525,10 @@
     </row>
     <row r="13" spans="1:13" ht="47" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F13" s="77" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G13" s="77" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H13" s="78" t="s">
         <v>2</v>
@@ -1565,7 +1559,7 @@
         <v>4</v>
       </c>
       <c r="G15" s="39"/>
-      <c r="H15" s="81">
+      <c r="H15" s="80">
         <f>SUM(H17:H122)</f>
         <v>0</v>
       </c>
@@ -6252,7 +6246,7 @@
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
@@ -6285,7 +6279,7 @@
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -6318,7 +6312,7 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
set up the company-object pairs
</commit_message>
<xml_diff>
--- a/v3/template.xlsx
+++ b/v3/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akha/Documents/api_excel/v3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78727B1A-D9C3-FF41-B26A-E7B77FD68119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4CEEAE-DB39-7D4C-8D85-D5D06858667F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15900" tabRatio="505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52800" yWindow="500" windowWidth="19200" windowHeight="19500" tabRatio="505" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REESTR" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="129">
   <si>
     <t>Дата:</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Риск-менеджер</t>
   </si>
   <si>
-    <t>Четтикбаев М.К.</t>
-  </si>
-  <si>
     <t>Директор по строительству</t>
   </si>
   <si>
@@ -360,6 +357,72 @@
   </si>
   <si>
     <t>РЕЕСТР Платежей №</t>
+  </si>
+  <si>
+    <t>Комеков М.К</t>
+  </si>
+  <si>
+    <t>Касымов Э.А.</t>
+  </si>
+  <si>
+    <t>ТОО "ДСК GLB"</t>
+  </si>
+  <si>
+    <t>ТОО «Аллея Тысячелетия»</t>
+  </si>
+  <si>
+    <t>ТОО "Алтын Шар West"</t>
+  </si>
+  <si>
+    <t>ТОО "Grand Victoria City"</t>
+  </si>
+  <si>
+    <t>ТОО "АльфаСтройПроект"</t>
+  </si>
+  <si>
+    <t>ТОО "Астана концепт"</t>
+  </si>
+  <si>
+    <t>ТОО "Дивный град"</t>
+  </si>
+  <si>
+    <t>ТОО "Строительное развитие Астана"</t>
+  </si>
+  <si>
+    <t>Жаукенов М.К.</t>
+  </si>
+  <si>
+    <t>Кусаинов Д.К.</t>
+  </si>
+  <si>
+    <t>ТОО "Проект Авангард"</t>
+  </si>
+  <si>
+    <t>ТОО "Интеграл Проект"</t>
+  </si>
+  <si>
+    <t>ТОО "ForwardProjekt"</t>
+  </si>
+  <si>
+    <t>ТОО "Проект Максимум"</t>
+  </si>
+  <si>
+    <t>ТОО "GrandNurProject"</t>
+  </si>
+  <si>
+    <t>ТОО "АстанаГрандПроект"</t>
+  </si>
+  <si>
+    <t>ТОО "Арнау Проект"</t>
+  </si>
+  <si>
+    <t>ТОО "NurAtakentStroy"</t>
+  </si>
+  <si>
+    <t>ТОО "НурКомИнжиниринг"</t>
+  </si>
+  <si>
+    <t>ТОО "Limon Project"</t>
   </si>
 </sst>
 </file>
@@ -511,7 +574,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -709,11 +772,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -916,14 +999,34 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="14" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1330,8 +1433,8 @@
   </sheetPr>
   <dimension ref="A1:R322"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView zoomScale="137" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1363,19 +1466,19 @@
     </row>
     <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="44"/>
-      <c r="B2" s="50" t="e">
+      <c r="B2" s="50">
         <f>INDEX(СПР_ОБЪЕКТОВ!$B$7:$K$80, MATCH($G11, СПР_ОБЪЕКТОВ!$B$7:$B$80, 0), 2)</f>
-        <v>#N/A</v>
+        <v>1</v>
       </c>
       <c r="C2" s="44"/>
-      <c r="F2" s="65" t="e">
+      <c r="F2" s="65" t="str">
         <f>IF(N($B2)=0,"","СОГЛАСОВАНО:")</f>
-        <v>#N/A</v>
+        <v>СОГЛАСОВАНО:</v>
       </c>
       <c r="G2" s="66"/>
       <c r="H2" s="67"/>
       <c r="I2" s="68" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J2" s="44"/>
       <c r="K2" s="44"/>
@@ -1386,15 +1489,15 @@
       <c r="A3" s="44"/>
       <c r="B3" s="45"/>
       <c r="C3" s="44"/>
-      <c r="F3" s="69" t="e">
-        <f>IF(N($B2)=0,"",VLOOKUP(N($B2),СПР_ПОДПИСАНТОВ!$B$8:$K$100,9,0)&amp;" "&amp;VLOOKUP(N($B2),СПР_ПОДПИСАНТОВ!$B$8:$K$100,7,0))</f>
-        <v>#N/A</v>
+      <c r="F3" s="69" t="str">
+        <f>IF(N($B2)=0,"",VLOOKUP(N($B2),СПР_ПОДПИСАНТОВ!$B$8:$K$92,9,0)&amp;" "&amp;VLOOKUP(N($B2),СПР_ПОДПИСАНТОВ!$B$8:$K$92,7,0))</f>
+        <v>Генеральный директор ТОО "Шар Құрылыс"</v>
       </c>
       <c r="G3" s="66"/>
       <c r="H3" s="67"/>
-      <c r="I3" s="70" t="e">
-        <f>IF(N($B4)=0,"",VLOOKUP(N($B4),СПР_ПОДПИСАНТОВ!$B$8:$K$100,9,0)&amp;" "&amp;VLOOKUP(N($B4),СПР_ПОДПИСАНТОВ!$B$8:$K$100,7,0))</f>
-        <v>#N/A</v>
+      <c r="I3" s="70" t="str">
+        <f>IF(N($B4)=0,"",VLOOKUP(N($B4),СПР_ПОДПИСАНТОВ!$B$8:$K$92,9,0)&amp;" "&amp;VLOOKUP(N($B4),СПР_ПОДПИСАНТОВ!$B$8:$K$92,7,0))</f>
+        <v>Генеральный директор ТОО "Аргон Строй"</v>
       </c>
       <c r="J3" s="44"/>
       <c r="K3" s="44"/>
@@ -1403,9 +1506,9 @@
     </row>
     <row r="4" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="44"/>
-      <c r="B4" s="50" t="e">
+      <c r="B4" s="50">
         <f>INDEX(СПР_ОБЪЕКТОВ!$B$7:$K$80, MATCH($G11, СПР_ОБЪЕКТОВ!$B$7:$B$80, 0), 3)</f>
-        <v>#N/A</v>
+        <v>17</v>
       </c>
       <c r="C4" s="44"/>
       <c r="F4" s="69"/>
@@ -1421,15 +1524,15 @@
       <c r="A5" s="44"/>
       <c r="B5" s="45"/>
       <c r="C5" s="44"/>
-      <c r="F5" s="69" t="e">
-        <f>IF(N($B2)=0,"","____________________________ "&amp;VLOOKUP(N($B2),СПР_ПОДПИСАНТОВ!$B$7:$K$100,5,0))</f>
-        <v>#N/A</v>
+      <c r="F5" s="69" t="str">
+        <f>IF(N($B2)=0,"","____________________________ "&amp;VLOOKUP(N($B2),СПР_ПОДПИСАНТОВ!$B$7:$K$92,5,0))</f>
+        <v>____________________________ Аманов Б.Ш.</v>
       </c>
       <c r="G5" s="66"/>
       <c r="H5" s="67"/>
-      <c r="I5" s="70" t="e">
-        <f>IF(N($B4)=0,"","____________________________ "&amp;VLOOKUP(N($B4),СПР_ПОДПИСАНТОВ!$B$8:$K$100,5,0))</f>
-        <v>#N/A</v>
+      <c r="I5" s="70" t="str">
+        <f>IF(N($B4)=0,"","____________________________ "&amp;VLOOKUP(N($B4),СПР_ПОДПИСАНТОВ!$B$8:$K$92,5,0))</f>
+        <v>____________________________ Билисбеков Н.Д.</v>
       </c>
       <c r="J5" s="44"/>
       <c r="K5" s="44"/>
@@ -1449,11 +1552,11 @@
       <c r="A7" s="52"/>
       <c r="B7" s="45"/>
       <c r="C7" s="52"/>
-      <c r="F7" s="83" t="s">
-        <v>107</v>
-      </c>
-      <c r="G7" s="84"/>
-      <c r="H7" s="85"/>
+      <c r="F7" s="82" t="s">
+        <v>106</v>
+      </c>
+      <c r="G7" s="83"/>
+      <c r="H7" s="84"/>
       <c r="I7" s="81"/>
       <c r="J7" s="52"/>
       <c r="K7" s="52"/>
@@ -1496,8 +1599,8 @@
       <c r="H10" s="67"/>
       <c r="I10" s="66"/>
       <c r="J10" s="29"/>
-      <c r="K10" s="82"/>
-      <c r="L10" s="82"/>
+      <c r="K10" s="93"/>
+      <c r="L10" s="93"/>
       <c r="M10" s="29"/>
     </row>
     <row r="11" spans="1:13" ht="19" thickBot="1" x14ac:dyDescent="0.25">
@@ -1509,7 +1612,9 @@
       <c r="F11" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="G11" s="74"/>
+      <c r="G11" s="74" t="s">
+        <v>103</v>
+      </c>
       <c r="H11" s="74"/>
       <c r="I11" s="75"/>
     </row>
@@ -1525,10 +1630,10 @@
     </row>
     <row r="13" spans="1:13" ht="47" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F13" s="77" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G13" s="77" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H13" s="78" t="s">
         <v>2</v>
@@ -5262,10 +5367,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:K49"/>
+  <dimension ref="A2:K59"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5483,7 +5588,7 @@
         <v>15</v>
       </c>
       <c r="G15" s="18">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H15" s="19" t="s">
         <v>16</v>
@@ -5541,13 +5646,13 @@
       <c r="D18" s="18"/>
       <c r="E18" s="18"/>
       <c r="F18" s="19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G18" s="18"/>
       <c r="H18" s="19"/>
       <c r="I18" s="18"/>
       <c r="J18" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K18" s="18"/>
     </row>
@@ -5566,7 +5671,7 @@
       <c r="H19" s="19"/>
       <c r="I19" s="18"/>
       <c r="J19" s="19" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K19" s="18"/>
     </row>
@@ -5579,13 +5684,13 @@
       <c r="D20" s="18"/>
       <c r="E20" s="18"/>
       <c r="F20" s="19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G20" s="18"/>
       <c r="H20" s="19"/>
       <c r="I20" s="18"/>
       <c r="J20" s="19" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K20" s="18"/>
     </row>
@@ -5598,13 +5703,13 @@
       <c r="D21" s="18"/>
       <c r="E21" s="18"/>
       <c r="F21" s="19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G21" s="18"/>
       <c r="H21" s="19"/>
       <c r="I21" s="18"/>
       <c r="J21" s="19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K21" s="18"/>
     </row>
@@ -5617,13 +5722,13 @@
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
       <c r="F22" s="19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G22" s="18"/>
       <c r="H22" s="19"/>
       <c r="I22" s="18"/>
       <c r="J22" s="19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K22" s="18"/>
     </row>
@@ -5635,14 +5740,14 @@
       <c r="C23" s="18"/>
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
-      <c r="F23" s="19" t="s">
-        <v>31</v>
+      <c r="F23" s="20" t="s">
+        <v>32</v>
       </c>
       <c r="G23" s="18"/>
       <c r="H23" s="19"/>
       <c r="I23" s="18"/>
       <c r="J23" s="19" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K23" s="18"/>
     </row>
@@ -5654,14 +5759,18 @@
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
       <c r="E24" s="18"/>
-      <c r="F24" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G24" s="18"/>
-      <c r="H24" s="19"/>
+      <c r="F24" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="G24" s="18">
+        <v>1</v>
+      </c>
+      <c r="H24" s="19" t="s">
+        <v>51</v>
+      </c>
       <c r="I24" s="18"/>
       <c r="J24" s="19" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="K24" s="18"/>
     </row>
@@ -5674,13 +5783,13 @@
       <c r="D25" s="18"/>
       <c r="E25" s="18"/>
       <c r="F25" s="20" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="G25" s="18">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="H25" s="19" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="I25" s="18"/>
       <c r="J25" s="19" t="s">
@@ -5696,14 +5805,14 @@
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
       <c r="E26" s="18"/>
-      <c r="F26" s="20" t="s">
-        <v>37</v>
+      <c r="F26" s="19" t="s">
+        <v>108</v>
       </c>
       <c r="G26" s="18">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="H26" s="19" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="I26" s="18"/>
       <c r="J26" s="19" t="s">
@@ -5719,14 +5828,14 @@
       <c r="C27" s="18"/>
       <c r="D27" s="18"/>
       <c r="E27" s="18"/>
-      <c r="F27" s="20" t="s">
-        <v>39</v>
+      <c r="F27" s="19" t="s">
+        <v>108</v>
       </c>
       <c r="G27" s="18">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H27" s="19" t="s">
-        <v>40</v>
+        <v>109</v>
       </c>
       <c r="I27" s="18"/>
       <c r="J27" s="19" t="s">
@@ -5742,14 +5851,14 @@
       <c r="C28" s="18"/>
       <c r="D28" s="18"/>
       <c r="E28" s="18"/>
-      <c r="F28" s="20" t="s">
-        <v>41</v>
+      <c r="F28" s="19" t="s">
+        <v>34</v>
       </c>
       <c r="G28" s="18">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="H28" s="19" t="s">
-        <v>42</v>
+        <v>110</v>
       </c>
       <c r="I28" s="18"/>
       <c r="J28" s="19" t="s">
@@ -5766,10 +5875,10 @@
       <c r="D29" s="18"/>
       <c r="E29" s="18"/>
       <c r="F29" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G29" s="18">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="H29" s="19" t="s">
         <v>43</v>
@@ -5788,14 +5897,14 @@
       <c r="C30" s="18"/>
       <c r="D30" s="18"/>
       <c r="E30" s="18"/>
-      <c r="F30" s="19" t="s">
-        <v>35</v>
+      <c r="F30" s="20" t="s">
+        <v>38</v>
       </c>
       <c r="G30" s="18">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H30" s="19" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I30" s="18"/>
       <c r="J30" s="19" t="s">
@@ -5811,14 +5920,14 @@
       <c r="C31" s="18"/>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
-      <c r="F31" s="19" t="s">
-        <v>35</v>
+      <c r="F31" s="20" t="s">
+        <v>36</v>
       </c>
       <c r="G31" s="18">
+        <v>9</v>
+      </c>
+      <c r="H31" s="19" t="s">
         <v>37</v>
-      </c>
-      <c r="H31" s="19" t="s">
-        <v>45</v>
       </c>
       <c r="I31" s="18"/>
       <c r="J31" s="19" t="s">
@@ -5835,13 +5944,13 @@
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
       <c r="F32" s="19" t="s">
-        <v>35</v>
+        <v>117</v>
       </c>
       <c r="G32" s="18">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>46</v>
+        <v>111</v>
       </c>
       <c r="I32" s="18"/>
       <c r="J32" s="19" t="s">
@@ -5858,13 +5967,13 @@
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
       <c r="F33" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G33" s="18">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="H33" s="19" t="s">
-        <v>47</v>
+        <v>112</v>
       </c>
       <c r="I33" s="18"/>
       <c r="J33" s="19" t="s">
@@ -5881,13 +5990,13 @@
       <c r="D34" s="18"/>
       <c r="E34" s="18"/>
       <c r="F34" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G34" s="18">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="H34" s="19" t="s">
-        <v>48</v>
+        <v>113</v>
       </c>
       <c r="I34" s="18"/>
       <c r="J34" s="19" t="s">
@@ -5904,13 +6013,13 @@
       <c r="D35" s="18"/>
       <c r="E35" s="18"/>
       <c r="F35" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G35" s="18">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="H35" s="19" t="s">
-        <v>49</v>
+        <v>114</v>
       </c>
       <c r="I35" s="18"/>
       <c r="J35" s="19" t="s">
@@ -5927,13 +6036,13 @@
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
       <c r="F36" s="19" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="G36" s="18">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="H36" s="19" t="s">
-        <v>51</v>
+        <v>115</v>
       </c>
       <c r="I36" s="18"/>
       <c r="J36" s="19" t="s">
@@ -5950,13 +6059,13 @@
       <c r="D37" s="18"/>
       <c r="E37" s="18"/>
       <c r="F37" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G37" s="18">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="H37" s="19" t="s">
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="I37" s="18"/>
       <c r="J37" s="19" t="s">
@@ -5973,13 +6082,13 @@
       <c r="D38" s="18"/>
       <c r="E38" s="18"/>
       <c r="F38" s="19" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="G38" s="18">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="H38" s="19" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="I38" s="18"/>
       <c r="J38" s="19" t="s">
@@ -5995,14 +6104,14 @@
       <c r="C39" s="18"/>
       <c r="D39" s="18"/>
       <c r="E39" s="18"/>
-      <c r="F39" s="20" t="s">
-        <v>54</v>
+      <c r="F39" s="19" t="s">
+        <v>49</v>
       </c>
       <c r="G39" s="18">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="H39" s="19" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="I39" s="18"/>
       <c r="J39" s="19" t="s">
@@ -6018,11 +6127,15 @@
       <c r="C40" s="18"/>
       <c r="D40" s="18"/>
       <c r="E40" s="18"/>
-      <c r="F40" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="G40" s="18"/>
-      <c r="H40" s="19"/>
+      <c r="F40" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G40" s="18">
+        <v>18</v>
+      </c>
+      <c r="H40" s="19" t="s">
+        <v>41</v>
+      </c>
       <c r="I40" s="18"/>
       <c r="J40" s="19" t="s">
         <v>17</v>
@@ -6031,123 +6144,432 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
-      <c r="B41" s="17"/>
+      <c r="B41" s="17">
+        <v>27</v>
+      </c>
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
       <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="19"/>
+      <c r="F41" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="G41" s="18">
+        <v>19</v>
+      </c>
+      <c r="H41" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="I41" s="18"/>
-      <c r="J41" s="19"/>
+      <c r="J41" s="19" t="s">
+        <v>17</v>
+      </c>
       <c r="K41" s="18"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
-      <c r="B42" s="17"/>
+      <c r="B42" s="17">
+        <v>28</v>
+      </c>
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="19"/>
+      <c r="F42" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G42" s="18">
+        <v>20</v>
+      </c>
+      <c r="H42" s="19" t="s">
+        <v>43</v>
+      </c>
       <c r="I42" s="18"/>
-      <c r="J42" s="19"/>
+      <c r="J42" s="19" t="s">
+        <v>17</v>
+      </c>
       <c r="K42" s="18"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
-      <c r="B43" s="17"/>
+      <c r="B43" s="17">
+        <v>29</v>
+      </c>
       <c r="C43" s="18"/>
       <c r="D43" s="18"/>
       <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="19"/>
+      <c r="F43" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G43" s="18">
+        <v>21</v>
+      </c>
+      <c r="H43" s="19" t="s">
+        <v>44</v>
+      </c>
       <c r="I43" s="18"/>
-      <c r="J43" s="19"/>
+      <c r="J43" s="19" t="s">
+        <v>17</v>
+      </c>
       <c r="K43" s="18"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
-      <c r="B44" s="17"/>
+      <c r="B44" s="17">
+        <v>30</v>
+      </c>
       <c r="C44" s="18"/>
       <c r="D44" s="18"/>
       <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="19"/>
+      <c r="F44" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G44" s="18">
+        <v>22</v>
+      </c>
+      <c r="H44" s="19" t="s">
+        <v>45</v>
+      </c>
       <c r="I44" s="18"/>
-      <c r="J44" s="19"/>
+      <c r="J44" s="19" t="s">
+        <v>17</v>
+      </c>
       <c r="K44" s="18"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
-      <c r="B45" s="17"/>
+      <c r="B45" s="17">
+        <v>31</v>
+      </c>
       <c r="C45" s="18"/>
       <c r="D45" s="18"/>
       <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
-      <c r="H45" s="19"/>
+      <c r="F45" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G45" s="18">
+        <v>23</v>
+      </c>
+      <c r="H45" s="19" t="s">
+        <v>46</v>
+      </c>
       <c r="I45" s="18"/>
-      <c r="J45" s="19"/>
+      <c r="J45" s="19" t="s">
+        <v>17</v>
+      </c>
       <c r="K45" s="18"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
-      <c r="B46" s="17"/>
+      <c r="B46" s="17">
+        <v>32</v>
+      </c>
       <c r="C46" s="18"/>
       <c r="D46" s="18"/>
       <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="19"/>
+      <c r="F46" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G46" s="18">
+        <v>24</v>
+      </c>
+      <c r="H46" s="19" t="s">
+        <v>47</v>
+      </c>
       <c r="I46" s="18"/>
-      <c r="J46" s="19"/>
+      <c r="J46" s="19" t="s">
+        <v>17</v>
+      </c>
       <c r="K46" s="18"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
-      <c r="B47" s="17"/>
+      <c r="B47" s="17">
+        <v>33</v>
+      </c>
       <c r="C47" s="18"/>
       <c r="D47" s="18"/>
       <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="19"/>
+      <c r="F47" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G47" s="18">
+        <v>25</v>
+      </c>
+      <c r="H47" s="19" t="s">
+        <v>48</v>
+      </c>
       <c r="I47" s="18"/>
-      <c r="J47" s="19"/>
+      <c r="J47" s="19" t="s">
+        <v>17</v>
+      </c>
       <c r="K47" s="18"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
-      <c r="B48" s="17"/>
+      <c r="B48" s="17">
+        <v>34</v>
+      </c>
       <c r="C48" s="18"/>
       <c r="D48" s="18"/>
       <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="19"/>
+      <c r="F48" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G48" s="18">
+        <v>26</v>
+      </c>
+      <c r="H48" s="19" t="s">
+        <v>119</v>
+      </c>
       <c r="I48" s="18"/>
-      <c r="J48" s="19"/>
+      <c r="J48" s="19" t="s">
+        <v>17</v>
+      </c>
       <c r="K48" s="18"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="18"/>
-      <c r="H49" s="19"/>
-      <c r="I49" s="18"/>
-      <c r="J49" s="18"/>
-      <c r="K49" s="18"/>
+      <c r="B49" s="85">
+        <v>35</v>
+      </c>
+      <c r="C49" s="86"/>
+      <c r="D49" s="86"/>
+      <c r="E49" s="86"/>
+      <c r="F49" s="87" t="s">
+        <v>34</v>
+      </c>
+      <c r="G49" s="86">
+        <v>27</v>
+      </c>
+      <c r="H49" s="87" t="s">
+        <v>120</v>
+      </c>
+      <c r="I49" s="86"/>
+      <c r="J49" s="87" t="s">
+        <v>17</v>
+      </c>
+      <c r="K49" s="86"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B50" s="92">
+        <v>36</v>
+      </c>
+      <c r="C50" s="88"/>
+      <c r="D50" s="88"/>
+      <c r="E50" s="89"/>
+      <c r="F50" s="89" t="s">
+        <v>34</v>
+      </c>
+      <c r="G50" s="90">
+        <v>28</v>
+      </c>
+      <c r="H50" s="89" t="s">
+        <v>121</v>
+      </c>
+      <c r="I50" s="88"/>
+      <c r="J50" s="91" t="s">
+        <v>17</v>
+      </c>
+      <c r="K50" s="89"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B51" s="90">
+        <v>37</v>
+      </c>
+      <c r="C51" s="90"/>
+      <c r="D51" s="90"/>
+      <c r="E51" s="90"/>
+      <c r="F51" s="91" t="s">
+        <v>34</v>
+      </c>
+      <c r="G51" s="90">
+        <v>29</v>
+      </c>
+      <c r="H51" s="91" t="s">
+        <v>35</v>
+      </c>
+      <c r="I51" s="90"/>
+      <c r="J51" s="91" t="s">
+        <v>17</v>
+      </c>
+      <c r="K51" s="90"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B52" s="17">
+        <v>38</v>
+      </c>
+      <c r="C52" s="18"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G52" s="18">
+        <v>30</v>
+      </c>
+      <c r="H52" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="I52" s="18"/>
+      <c r="J52" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="K52" s="18"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B53" s="17">
+        <v>39</v>
+      </c>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G53" s="18">
+        <v>31</v>
+      </c>
+      <c r="H53" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="I53" s="18"/>
+      <c r="J53" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="K53" s="18"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B54" s="17">
+        <v>40</v>
+      </c>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G54" s="18">
+        <v>32</v>
+      </c>
+      <c r="H54" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="I54" s="18"/>
+      <c r="J54" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="K54" s="18"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B55" s="17">
+        <v>41</v>
+      </c>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G55" s="18">
+        <v>33</v>
+      </c>
+      <c r="H55" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="I55" s="18"/>
+      <c r="J55" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="K55" s="18"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B56" s="17">
+        <v>42</v>
+      </c>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G56" s="18">
+        <v>34</v>
+      </c>
+      <c r="H56" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="I56" s="18"/>
+      <c r="J56" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="K56" s="18"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B57" s="17">
+        <v>43</v>
+      </c>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G57" s="18">
+        <v>35</v>
+      </c>
+      <c r="H57" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="I57" s="18"/>
+      <c r="J57" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="K57" s="18"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B58" s="17">
+        <v>44</v>
+      </c>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G58" s="18">
+        <v>36</v>
+      </c>
+      <c r="H58" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="I58" s="18"/>
+      <c r="J58" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="K58" s="18"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B59" s="17">
+        <v>45</v>
+      </c>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G59" s="18">
+        <v>37</v>
+      </c>
+      <c r="H59" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="I59" s="18"/>
+      <c r="J59" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="K59" s="18"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="uMsdPwTQeexHyohCDNuIfC+a/3/HO7llseO6psVrMLjqrOO1Zdl8f7ibFlr3WgnIMSCH0ms/TyKj4VlrpTFQIw==" saltValue="rYzlr/gIVgA/p7ukV/FVYQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
@@ -6161,8 +6583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A4:N63"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:K12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="134" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6174,61 +6596,61 @@
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="N4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="21" t="s">
         <v>57</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="C6" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="E6" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="F6" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="G6" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="H6" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="I6" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="J6" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="J6" s="22" t="s">
+      <c r="K6" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="K6" s="22" t="s">
+      <c r="L6" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="L6" s="22" t="s">
+      <c r="M6" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="M6" s="22" t="s">
+      <c r="N6" s="22" t="s">
         <v>69</v>
-      </c>
-      <c r="N6" s="22" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" s="23"/>
       <c r="D7" s="23"/>
@@ -6246,7 +6668,10 @@
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
@@ -6279,7 +6704,10 @@
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -6312,13 +6740,13 @@
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
       </c>
       <c r="D10" s="1">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E10" s="1">
         <v>2</v>
@@ -6342,7 +6770,10 @@
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
@@ -6375,7 +6806,10 @@
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
@@ -6408,7 +6842,10 @@
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
@@ -6441,7 +6878,10 @@
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
@@ -6474,7 +6914,10 @@
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
@@ -6507,7 +6950,10 @@
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
@@ -6540,7 +6986,10 @@
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
@@ -6573,7 +7022,10 @@
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
@@ -6606,7 +7058,10 @@
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
@@ -6639,7 +7094,10 @@
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
@@ -6672,7 +7130,10 @@
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="25" t="s">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
@@ -6705,7 +7166,10 @@
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
@@ -6738,7 +7202,7 @@
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="N23" s="1">
         <v>3</v>
@@ -6747,7 +7211,10 @@
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
       </c>
       <c r="D24" s="1">
         <v>1</v>
@@ -6777,7 +7244,10 @@
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="25" t="s">
-        <v>86</v>
+        <v>85</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
@@ -6807,7 +7277,7 @@
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
@@ -6843,9 +7313,11 @@
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="61" t="s">
-        <v>87</v>
-      </c>
-      <c r="C27" s="62"/>
+        <v>86</v>
+      </c>
+      <c r="C27" s="62">
+        <v>0</v>
+      </c>
       <c r="D27" s="63">
         <v>1</v>
       </c>
@@ -6879,9 +7351,11 @@
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="61" t="s">
-        <v>88</v>
-      </c>
-      <c r="C28" s="62"/>
+        <v>87</v>
+      </c>
+      <c r="C28" s="62">
+        <v>0</v>
+      </c>
       <c r="D28" s="63">
         <v>1</v>
       </c>
@@ -6915,7 +7389,10 @@
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0</v>
       </c>
       <c r="D29" s="1">
         <v>1</v>
@@ -6951,7 +7428,7 @@
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N31" s="1">
         <v>3</v>
@@ -6960,7 +7437,7 @@
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N32" s="1">
         <v>3</v>
@@ -6969,7 +7446,7 @@
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N33" s="1">
         <v>3</v>
@@ -6978,7 +7455,7 @@
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N34" s="1">
         <v>3</v>
@@ -6987,7 +7464,7 @@
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N35" s="1">
         <v>3</v>
@@ -6996,7 +7473,7 @@
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N36" s="1">
         <v>3</v>
@@ -7005,7 +7482,7 @@
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N37" s="1">
         <v>3</v>
@@ -7014,7 +7491,7 @@
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="25" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N38" s="1">
         <v>3</v>
@@ -7023,7 +7500,7 @@
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N39" s="1">
         <v>3</v>
@@ -7032,7 +7509,7 @@
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N40" s="1">
         <v>3</v>

</xml_diff>